<commit_message>
Rough Draft BDM Instructions
</commit_message>
<xml_diff>
--- a/BDM/BDMQs.xlsx
+++ b/BDM/BDMQs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\University Vivikth\Documents\UNI\Fourth Year\Thesis\Otree\Experimental_RET - Copy\BDM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D71D71-31DD-405E-A6C9-E52AA010DE85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF302329-7B9F-4087-A0EF-FC0254B843D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -76,21 +76,12 @@
     <t>D</t>
   </si>
   <si>
-    <t>I used the BDM procedure to determine how much Simon values an ice-cream in terms of the probability of leaving the experiment right now. Simon stated that his switch-point is 60%. From this, we can infer:</t>
-  </si>
-  <si>
     <t>Mishika must pick between a toy and some money. She would prefer the toy to $3, and prefer $5 to the toy. Suppose Mishika is given $4. Which of the following can we conclude?</t>
   </si>
   <si>
-    <t>I used the BDM procedure to determine how much Kriti values a mug in terms of the probability of leaving the experiment right now. Suppose Kriti states that her switch-point for 1 mug is 100%,and her switch point for 2 mugs is also 100%. Kriti also (truthfully) states that she prefers 2 mugs to 1 mug. What can we infer?</t>
-  </si>
-  <si>
     <t>I used the BDM procedure to determine how much Christian values a muesli bar in terms of money. Christian is allergic to nuts, and so prefers any amount of money to a muesli bar. What can we infer about Christian’s switch-point?</t>
   </si>
   <si>
-    <t>I used the BDM procedure to determine how much Borys and Sabi value a coffee in terms of the probability of leaving the experiment right now. Borys stated his switch-point was 25%, while Sabi stated his switch point was 50%. Both Borys and Sabi prefer leaving the experiment right now to not leaving the experiment right now. What can we infer?</t>
-  </si>
-  <si>
     <t>Sally’s lie will affect the experimental results</t>
   </si>
   <si>
@@ -152,6 +143,15 @@
   </si>
   <si>
     <t>Simon is indifferent between leaving the experiment right now and an ice-cream</t>
+  </si>
+  <si>
+    <t>I used the BDM procedure to determine how much Simon values an ice-cream in terms of the lottery (i.e case 2). Simon (truthfully) stated that his switch-point is 60%. From this, we can infer:</t>
+  </si>
+  <si>
+    <t>I used the BDM procedure to determine how much Borys and Sabi value a coffee in terms of the probability of leaving the experiment right now. Borys stated his switch-point was 25%, while Sabi stated his switch point was 50%. Both Borys and Sabi prefer leaving the experiment right now to reading the boring information. What can we infer?</t>
+  </si>
+  <si>
+    <t>I used the BDM procedure to determine how much Kriti values a mug in terms of the lottery (i.e case 2). Suppose Kriti states that her switch-point for 1 mug is 100%,and her switch point for 2 mugs is also 100%. Kriti also (truthfully) states that she prefers 2 mugs to 1 mug. What can we infer?</t>
   </si>
 </sst>
 </file>
@@ -998,7 +998,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1055,10 +1055,10 @@
         <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>13</v>
@@ -1072,16 +1072,16 @@
     </row>
     <row r="4" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>14</v>
@@ -1090,18 +1090,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>10</v>
@@ -1112,16 +1112,16 @@
     </row>
     <row r="6" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>10</v>
@@ -1132,19 +1132,19 @@
     </row>
     <row r="7" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>17</v>
@@ -1152,19 +1152,19 @@
     </row>
     <row r="8" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>11</v>
@@ -1173,19 +1173,19 @@
     </row>
     <row r="9" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="D9" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Tidied up BDM info
</commit_message>
<xml_diff>
--- a/BDM/BDMQs.xlsx
+++ b/BDM/BDMQs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\University Vivikth\Documents\UNI\Fourth Year\Thesis\Otree\Experimental_RET - Copy\BDM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39A3741-A61E-4197-8E9D-ACE0E688F066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB7C60C-CBBF-41C1-A580-FA2213A3AA9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>question</t>
   </si>
@@ -40,27 +40,12 @@
     <t>solution</t>
   </si>
   <si>
-    <t>Evan’s switch-point for 2 cheeseburgers would be higher than $10</t>
-  </si>
-  <si>
-    <t>Evan’s switch-point for 2 cheeseburgers would be lower than $10</t>
-  </si>
-  <si>
-    <t>Evan’s switch-point for 2 cheeseburgers would be equal to $10</t>
-  </si>
-  <si>
-    <t>There is not enough information to pick one of the above</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
     <t>B</t>
   </si>
   <si>
-    <t>Sally won’t get her preferred outcome if the question she lied on is randomly selected</t>
-  </si>
-  <si>
     <t>Sally will spend more time in the experiment</t>
   </si>
   <si>
@@ -73,21 +58,12 @@
     <t>Mishika must pick between a toy and some money. She would prefer the toy to $3, and prefer $5 to the toy. Suppose Mishika is given $4. Which of the following can we conclude?</t>
   </si>
   <si>
-    <t>Sally’s lie will affect the experimental results</t>
-  </si>
-  <si>
     <t>There are no negative consequences associated with lying for Sally</t>
   </si>
   <si>
     <t>Sally may not always get her preferred outcome</t>
   </si>
   <si>
-    <t>Kriti prefers 2 mugs to leaving the experiment right now</t>
-  </si>
-  <si>
-    <t>Kriti prefers leaving the experiment right now to 1 mug</t>
-  </si>
-  <si>
     <t>Christian’s switch-point is less than $2</t>
   </si>
   <si>
@@ -100,18 +76,6 @@
     <t>Christian’s switch-point is equal to $2</t>
   </si>
   <si>
-    <t>Simon prefers leaving the experiment right now to an ice-cream</t>
-  </si>
-  <si>
-    <t>Simon prefers an ice-cream to leaving the experiment right now</t>
-  </si>
-  <si>
-    <t>Kriti prefers 1 mug to 2 mugs</t>
-  </si>
-  <si>
-    <t>Simon is indifferent between leaving the experiment right now and an ice-cream</t>
-  </si>
-  <si>
     <t>Sabi receives $5, which he prefers to the soft drink</t>
   </si>
   <si>
@@ -133,33 +97,9 @@
     <t>Borys receives the pizza, but would prefer the 80% lottery</t>
   </si>
   <si>
-    <t>If Jack prefers leaving the experiment immediately to reading the boring information and continuing with the experiment, then Jack prefers the spoon to the fork</t>
-  </si>
-  <si>
-    <t>If Jack prefers leaving the experiment immediately to reading the boring information and continuing with the experiment, then Jack prefers the fork to the spoon</t>
-  </si>
-  <si>
-    <t>If Jack does not prefer leaving the experiment immediately to reading the boring information and continuing with the experiment, then Jack prefers the spoon to the fork</t>
-  </si>
-  <si>
-    <t>If Jack does not prefer leaving the experiment immediately to reading the boring information and continuing with the experiment, then Jack prefers the fork to the spoon</t>
-  </si>
-  <si>
-    <t>I used the monetary switch-point procedure to determine how much Evan values a cheeseburger. Evan said that his switch point for a single cheeseburger was $10. Evan also stated (truthfully) that he prefers more cheeseburgers to less. Which of the following is true?</t>
-  </si>
-  <si>
     <t>I used the lottery switch-point procedure to determine how much Sally values a chocolate bar. Which of the following is a potential negative outcome for Sally if she lies about her switch-point?</t>
   </si>
   <si>
-    <t>I used the pseudo switch-point procedure to determine how much Sally values a chocolate bar. Which of the following is a potential negative outcome for Sally if she lies on one of the questions?</t>
-  </si>
-  <si>
-    <t>I used the lottery switch-point procedure to determine how much Simon values an ice-cream). Simon (truthfully) stated that his switch-point is 60%. From this, we can infer:</t>
-  </si>
-  <si>
-    <t>I used the lottery switch-point procedure to determine how much Kriti values a mug. Suppose Kriti states that her switch-point for 1 mug is 100%,and her switch point for 2 mugs is also 100%. Kriti also (truthfully) states that she prefers 2 mugs to 1 mug. What can we infer?</t>
-  </si>
-  <si>
     <t>She would be happier if she received the toy, as her monetary switch point is $5</t>
   </si>
   <si>
@@ -181,10 +121,10 @@
     <t>I used the lottery switch-point procedure to determine how much Borys values a pizza. His true switch-point is 70%, but he lied and told me his switch-point is 50%. What happens if I randomly select question 81 (which corresponds to 80%)?</t>
   </si>
   <si>
-    <t>I used the lottery switch-point procedure to determine Jack's switch-points for a spoon and a fork. Jack told me (truthfully) that his switch-point  for a spoon is 40%, and his switch-point for a fork is 70%.  Which of the following is correct?</t>
-  </si>
-  <si>
     <t>Sabi receives the soft-drink, which he prefers to $5</t>
+  </si>
+  <si>
+    <t>Both of the above options</t>
   </si>
 </sst>
 </file>
@@ -1028,10 +968,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1063,206 +1003,146 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>11</v>
-      </c>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
@@ -1280,46 +1160,6 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated BDM data for ease of use
</commit_message>
<xml_diff>
--- a/BDM/BDMQs.xlsx
+++ b/BDM/BDMQs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\University Vivikth\Documents\UNI\Fourth Year\Thesis\Otree\Experimental_RET - Copy\BDM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE136CC-0B6C-4B4F-989B-D4064F57F5BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C67F65E-0170-4FC8-9B88-00D58C960E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>question</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>I used the monetary switch-point procedure to determine how much Sabi values a soft drink. Sabi's true switch-point is $4, but he lied and told me his switch-point is $6. What happens if I randomly select question 5001 (which corresponds to $5)?</t>
+  </si>
+  <si>
+    <t>Qnum</t>
   </si>
 </sst>
 </file>
@@ -971,7 +974,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1002,6 +1005,9 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1022,6 +1028,9 @@
       <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -1042,6 +1051,9 @@
       <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1062,7 +1074,9 @@
       <c r="F4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="1"/>
+      <c r="G4" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -1083,6 +1097,9 @@
       <c r="F5" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -1102,6 +1119,9 @@
       </c>
       <c r="F6" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>